<commit_message>
Changed delimeter from _ to .
</commit_message>
<xml_diff>
--- a/Nautobot-tables.xlsx
+++ b/Nautobot-tables.xlsx
@@ -8,13 +8,13 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dcim_device-roles" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dcim_device-types" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dcim_manufacturers" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dcim_regions" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dcim_sites" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="users_tokens" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="users_users" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dcim.device-roles" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dcim.device-types" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dcim.manufacturers" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dcim.regions" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dcim.sites" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="users.tokens" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="users.users" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1002,12 +1002,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>db4449b0-0e6e-4c38-8086-3ff250a31bfa</t>
+          <t>f978e5c3-3836-4a26-bf9b-1f04b7a6e4ae</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://192.168.248.144:8080/api/dcim/regions/db4449b0-0e6e-4c38-8086-3ff250a31bfa/</t>
+          <t>http://192.168.248.144:8080/api/dcim/regions/f978e5c3-3836-4a26-bf9b-1f04b7a6e4ae/</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1030,12 +1030,12 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2022-05-12T05:43:10.442360Z</t>
+          <t>2022-05-13T04:25:40.319031Z</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -1047,12 +1047,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>e1edc03e-ab60-4b6e-bd3b-b1fd3503820e</t>
+          <t>271c8d66-8f2d-4bf0-85f8-62b3989afe11</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://192.168.248.144:8080/api/dcim/regions/e1edc03e-ab60-4b6e-bd3b-b1fd3503820e/</t>
+          <t>http://192.168.248.144:8080/api/dcim/regions/271c8d66-8f2d-4bf0-85f8-62b3989afe11/</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1075,12 +1075,12 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2022-05-12T05:43:10.452839Z</t>
+          <t>2022-05-13T04:25:40.331620Z</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -1092,12 +1092,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>686a79d7-4d4b-4fa1-8331-56fdf842b290</t>
+          <t>21b0dcc7-4c24-489e-8f82-4d8cdcfdd545</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://192.168.248.144:8080/api/dcim/regions/686a79d7-4d4b-4fa1-8331-56fdf842b290/</t>
+          <t>http://192.168.248.144:8080/api/dcim/regions/21b0dcc7-4c24-489e-8f82-4d8cdcfdd545/</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1120,12 +1120,12 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2022-05-12T05:43:10.468447Z</t>
+          <t>2022-05-13T04:25:40.349150Z</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -1137,12 +1137,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>c449b305-3d1a-406c-8689-47d4a5d5b9b3</t>
+          <t>43832989-d85a-459e-9ce3-741407cd76c6</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://192.168.248.144:8080/api/dcim/regions/c449b305-3d1a-406c-8689-47d4a5d5b9b3/</t>
+          <t>http://192.168.248.144:8080/api/dcim/regions/43832989-d85a-459e-9ce3-741407cd76c6/</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1165,12 +1165,12 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2022-05-12T05:43:10.460496Z</t>
+          <t>2022-05-13T04:25:40.339997Z</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -1182,12 +1182,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>a483f747-b92b-4b3b-94d5-9fad13d92132</t>
+          <t>20b54a29-6268-4e79-859d-a54d60fe4c95</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://192.168.248.144:8080/api/dcim/regions/a483f747-b92b-4b3b-94d5-9fad13d92132/</t>
+          <t>http://192.168.248.144:8080/api/dcim/regions/20b54a29-6268-4e79-859d-a54d60fe4c95/</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1210,12 +1210,12 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2022-05-12T05:43:10.476166Z</t>
+          <t>2022-05-13T04:25:40.357922Z</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1398,12 +1398,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>7e98eec7-7536-43de-8106-5f0fc0277771</t>
+          <t>fb29f887-28be-490f-b935-dd3ff3b2c81e</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://192.168.248.144:8080/api/dcim/sites/7e98eec7-7536-43de-8106-5f0fc0277771/</t>
+          <t>http://192.168.248.144:8080/api/dcim/sites/fb29f887-28be-490f-b935-dd3ff3b2c81e/</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>db4449b0-0e6e-4c38-8086-3ff250a31bfa</t>
+          <t>f978e5c3-3836-4a26-bf9b-1f04b7a6e4ae</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -1442,12 +1442,12 @@
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>2022-05-12T05:43:10.528886Z</t>
+          <t>2022-05-13T04:25:40.420468Z</t>
         </is>
       </c>
       <c r="X2" t="n">
@@ -1477,12 +1477,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>bfda455e-186a-4358-822e-364f93a6249a</t>
+          <t>6064d233-ed27-4436-b964-f676d47765d2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://192.168.248.144:8080/api/dcim/sites/bfda455e-186a-4358-822e-364f93a6249a/</t>
+          <t>http://192.168.248.144:8080/api/dcim/sites/6064d233-ed27-4436-b964-f676d47765d2/</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>db4449b0-0e6e-4c38-8086-3ff250a31bfa</t>
+          <t>f978e5c3-3836-4a26-bf9b-1f04b7a6e4ae</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -1521,12 +1521,12 @@
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>2022-05-12T05:43:10.540562Z</t>
+          <t>2022-05-13T04:25:40.433948Z</t>
         </is>
       </c>
       <c r="X3" t="n">
@@ -1556,12 +1556,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>9434d7b8-6769-4add-a256-944bc6b55796</t>
+          <t>c75e17a0-6b4a-4faf-9ce1-65c9967e825a</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://192.168.248.144:8080/api/dcim/sites/9434d7b8-6769-4add-a256-944bc6b55796/</t>
+          <t>http://192.168.248.144:8080/api/dcim/sites/c75e17a0-6b4a-4faf-9ce1-65c9967e825a/</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>db4449b0-0e6e-4c38-8086-3ff250a31bfa</t>
+          <t>f978e5c3-3836-4a26-bf9b-1f04b7a6e4ae</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -1600,12 +1600,12 @@
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>2022-05-12T05:43:10.550238Z</t>
+          <t>2022-05-13T04:25:40.444607Z</t>
         </is>
       </c>
       <c r="X4" t="n">
@@ -1635,12 +1635,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>39e90cbf-c010-4d6e-8703-174d773a9fea</t>
+          <t>a0fba41c-ee34-4b94-a92b-518867e4ec50</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://192.168.248.144:8080/api/dcim/sites/39e90cbf-c010-4d6e-8703-174d773a9fea/</t>
+          <t>http://192.168.248.144:8080/api/dcim/sites/a0fba41c-ee34-4b94-a92b-518867e4ec50/</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>db4449b0-0e6e-4c38-8086-3ff250a31bfa</t>
+          <t>f978e5c3-3836-4a26-bf9b-1f04b7a6e4ae</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -1679,12 +1679,12 @@
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>2022-05-12T05:43:10.561011Z</t>
+          <t>2022-05-13T04:25:40.455912Z</t>
         </is>
       </c>
       <c r="X5" t="n">

</xml_diff>